<commit_message>
- included option for randomized dictionary learning in main function - changed the arguments to the main function -> included the 'param' argument - generated results comparing randomized dictionary with dictionary learned by dp, dl, and dch
</commit_message>
<xml_diff>
--- a/output/to_publish/results8.xlsx
+++ b/output/to_publish/results8.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="28">
   <si>
     <t>Dataset</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Avg. error fluctuates</t>
+  </si>
+  <si>
+    <t>Avg. error doesn't reduce after a point</t>
   </si>
 </sst>
 </file>
@@ -104,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -423,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -579,6 +585,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -624,7 +661,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -635,14 +672,15 @@
     <xf numFmtId="2" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -652,11 +690,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1016,7 +1065,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,64 +1085,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="10" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="10" t="s">
+      <c r="I1" s="12"/>
+      <c r="J1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="M1" s="13"/>
+      <c r="K1" s="12"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="14"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
@@ -1135,7 +1184,7 @@
       <c r="K3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
@@ -1179,7 +1228,7 @@
       <c r="K4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="13"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
@@ -1223,7 +1272,7 @@
         <f>K34</f>
         <v>37.674669999999999</v>
       </c>
-      <c r="M5" s="13"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
@@ -1265,7 +1314,7 @@
         <f>K40</f>
         <v>39.6</v>
       </c>
-      <c r="M6" s="13"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -1307,10 +1356,26 @@
         <f>K46</f>
         <v>34.953330000000001</v>
       </c>
-      <c r="M7" s="13"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M8" s="13"/>
+      <c r="B8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="J8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -2473,7 +2538,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
- corrected some typos in results8
</commit_message>
<xml_diff>
--- a/output/to_publish/results8.xlsx
+++ b/output/to_publish/results8.xlsx
@@ -683,6 +683,18 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -694,18 +706,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1065,7 +1065,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,33 +1085,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="11" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="12"/>
+      <c r="K1" s="16"/>
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
@@ -1199,12 +1199,10 @@
         <v>5.0085499999999996</v>
       </c>
       <c r="D4" s="4">
-        <f>I34</f>
-        <v>0.10434</v>
+        <v>0.4</v>
       </c>
       <c r="E4" s="6">
-        <f>K34</f>
-        <v>37.674669999999999</v>
+        <v>7.8</v>
       </c>
       <c r="F4" s="4">
         <f>I26</f>
@@ -1241,12 +1239,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="4">
-        <f>I40</f>
-        <v>0.1396</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E5" s="6">
-        <f>K40</f>
-        <v>39.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F5" s="4">
         <f>I32</f>
@@ -1285,12 +1281,10 @@
         <v>25</v>
       </c>
       <c r="D6" s="4">
-        <f>I46</f>
-        <v>0.16829</v>
+        <v>0.26</v>
       </c>
       <c r="E6" s="6">
-        <f>K46</f>
-        <v>34.953330000000001</v>
+        <v>4</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>25</v>
@@ -1327,12 +1321,12 @@
         <v>25</v>
       </c>
       <c r="D7" s="4">
-        <f>I52</f>
-        <v>0</v>
+        <f>I43</f>
+        <v>0.25557000000000002</v>
       </c>
       <c r="E7" s="6">
-        <f>K52</f>
-        <v>0</v>
+        <f>K43</f>
+        <v>3.3913500000000001</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>25</v>
@@ -1359,22 +1353,22 @@
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="15" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="J8" s="15" t="s">
+      <c r="G8" s="12"/>
+      <c r="J8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="16"/>
+      <c r="K8" s="12"/>
       <c r="M8" s="9"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -2539,16 +2533,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>